<commit_message>
add rounding to task_1d
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_d.xlsx
+++ b/data/fabian/output/processed_d.xlsx
@@ -460,13 +460,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4.073</v>
+        <v>4.07</v>
       </c>
       <c r="C2" t="n">
-        <v>6.908</v>
+        <v>6.91</v>
       </c>
       <c r="D2" t="n">
-        <v>1.087</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.331</v>
+        <v>3.33</v>
       </c>
       <c r="C3" t="n">
         <v>5.93</v>
       </c>
       <c r="D3" t="n">
-        <v>1.237</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.447</v>
+        <v>3.45</v>
       </c>
       <c r="C4" t="n">
-        <v>6.019</v>
+        <v>6.02</v>
       </c>
       <c r="D4" t="n">
-        <v>1.044</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.057</v>
+        <v>3.06</v>
       </c>
       <c r="C5" t="n">
-        <v>5.175</v>
+        <v>5.17</v>
       </c>
       <c r="D5" t="n">
-        <v>1.054</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.085</v>
+        <v>3.09</v>
       </c>
       <c r="C6" t="n">
-        <v>5.601</v>
+        <v>5.6</v>
       </c>
       <c r="D6" t="n">
-        <v>1.236</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.888</v>
+        <v>2.89</v>
       </c>
       <c r="C7" t="n">
-        <v>5.079</v>
+        <v>5.08</v>
       </c>
       <c r="D7" t="n">
-        <v>1.032</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.232</v>
+        <v>3.23</v>
       </c>
       <c r="C8" t="n">
-        <v>5.305</v>
+        <v>5.3</v>
       </c>
       <c r="D8" t="n">
-        <v>1.026</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.016</v>
+        <v>3.02</v>
       </c>
       <c r="C9" t="n">
-        <v>5.299</v>
+        <v>5.3</v>
       </c>
       <c r="D9" t="n">
-        <v>1.246</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2.768</v>
+        <v>2.77</v>
       </c>
       <c r="C10" t="n">
-        <v>4.933</v>
+        <v>4.93</v>
       </c>
       <c r="D10" t="n">
-        <v>0.974</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="11">
@@ -589,10 +589,10 @@
         <v>3.44</v>
       </c>
       <c r="C11" t="n">
-        <v>5.439</v>
+        <v>5.44</v>
       </c>
       <c r="D11" t="n">
-        <v>0.891</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3.178</v>
+        <v>3.18</v>
       </c>
       <c r="C12" t="n">
-        <v>5.589</v>
+        <v>5.59</v>
       </c>
       <c r="D12" t="n">
-        <v>1.533</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2.469</v>
+        <v>2.47</v>
       </c>
       <c r="C13" t="n">
-        <v>4.361</v>
+        <v>4.36</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="14">
@@ -631,10 +631,10 @@
         <v>2.67</v>
       </c>
       <c r="C14" t="n">
-        <v>4.284</v>
+        <v>4.28</v>
       </c>
       <c r="D14" t="n">
-        <v>0.596</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.694</v>
+        <v>2.69</v>
       </c>
       <c r="C15" t="n">
-        <v>4.508</v>
+        <v>4.51</v>
       </c>
       <c r="D15" t="n">
-        <v>0.729</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="16">
@@ -656,10 +656,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.283</v>
+        <v>2.28</v>
       </c>
       <c r="C16" t="n">
-        <v>3.818</v>
+        <v>3.82</v>
       </c>
       <c r="D16" t="n">
         <v>0.58</v>
@@ -670,10 +670,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.283</v>
+        <v>2.28</v>
       </c>
       <c r="C17" t="n">
-        <v>3.818</v>
+        <v>3.82</v>
       </c>
       <c r="D17" t="n">
         <v>0.58</v>
@@ -684,13 +684,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.694</v>
+        <v>2.69</v>
       </c>
       <c r="C18" t="n">
-        <v>4.508</v>
+        <v>4.51</v>
       </c>
       <c r="D18" t="n">
-        <v>0.729</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="19">
@@ -701,10 +701,10 @@
         <v>2.67</v>
       </c>
       <c r="C19" t="n">
-        <v>4.284</v>
+        <v>4.28</v>
       </c>
       <c r="D19" t="n">
-        <v>0.596</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.469</v>
+        <v>2.47</v>
       </c>
       <c r="C20" t="n">
-        <v>4.361</v>
+        <v>4.36</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>3.178</v>
+        <v>3.18</v>
       </c>
       <c r="C21" t="n">
-        <v>5.589</v>
+        <v>5.59</v>
       </c>
       <c r="D21" t="n">
-        <v>1.533</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="22">
@@ -743,10 +743,10 @@
         <v>3.44</v>
       </c>
       <c r="C22" t="n">
-        <v>5.439</v>
+        <v>5.44</v>
       </c>
       <c r="D22" t="n">
-        <v>0.891</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2.768</v>
+        <v>2.77</v>
       </c>
       <c r="C23" t="n">
-        <v>4.933</v>
+        <v>4.93</v>
       </c>
       <c r="D23" t="n">
-        <v>0.974</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>3.016</v>
+        <v>3.02</v>
       </c>
       <c r="C24" t="n">
-        <v>5.299</v>
+        <v>5.3</v>
       </c>
       <c r="D24" t="n">
-        <v>1.246</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.232</v>
+        <v>3.23</v>
       </c>
       <c r="C25" t="n">
-        <v>5.305</v>
+        <v>5.3</v>
       </c>
       <c r="D25" t="n">
-        <v>1.026</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2.888</v>
+        <v>2.89</v>
       </c>
       <c r="C26" t="n">
-        <v>5.079</v>
+        <v>5.08</v>
       </c>
       <c r="D26" t="n">
-        <v>1.032</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.085</v>
+        <v>3.09</v>
       </c>
       <c r="C27" t="n">
-        <v>5.601</v>
+        <v>5.6</v>
       </c>
       <c r="D27" t="n">
-        <v>1.236</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3.057</v>
+        <v>3.06</v>
       </c>
       <c r="C28" t="n">
-        <v>5.175</v>
+        <v>5.17</v>
       </c>
       <c r="D28" t="n">
-        <v>1.054</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>3.447</v>
+        <v>3.45</v>
       </c>
       <c r="C29" t="n">
-        <v>6.019</v>
+        <v>6.02</v>
       </c>
       <c r="D29" t="n">
-        <v>1.044</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>3.331</v>
+        <v>3.33</v>
       </c>
       <c r="C30" t="n">
         <v>5.93</v>
       </c>
       <c r="D30" t="n">
-        <v>1.237</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>4.073</v>
+        <v>4.07</v>
       </c>
       <c r="C31" t="n">
-        <v>6.908</v>
+        <v>6.91</v>
       </c>
       <c r="D31" t="n">
-        <v>1.087</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>4.549</v>
+        <v>4.55</v>
       </c>
       <c r="C32" t="n">
-        <v>6.285</v>
+        <v>6.28</v>
       </c>
       <c r="D32" t="n">
-        <v>10.607</v>
+        <v>10.61</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>5.005</v>
+        <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>5.985</v>
+        <v>5.98</v>
       </c>
       <c r="D33" t="n">
-        <v>10.009</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>42</v>
       </c>
       <c r="B34" t="n">
-        <v>4.434</v>
+        <v>4.43</v>
       </c>
       <c r="C34" t="n">
         <v>6.14</v>
       </c>
       <c r="D34" t="n">
-        <v>7.788</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>4.346</v>
+        <v>4.35</v>
       </c>
       <c r="C35" t="n">
-        <v>6.892</v>
+        <v>6.89</v>
       </c>
       <c r="D35" t="n">
-        <v>11.766</v>
+        <v>11.77</v>
       </c>
     </row>
     <row r="36">
@@ -936,10 +936,10 @@
         <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>4.145</v>
+        <v>4.15</v>
       </c>
       <c r="C36" t="n">
-        <v>6.548</v>
+        <v>6.55</v>
       </c>
       <c r="D36" t="n">
         <v>8.289999999999999</v>
@@ -950,13 +950,13 @@
         <v>45</v>
       </c>
       <c r="B37" t="n">
-        <v>4.149</v>
+        <v>4.15</v>
       </c>
       <c r="C37" t="n">
-        <v>6.564</v>
+        <v>6.56</v>
       </c>
       <c r="D37" t="n">
-        <v>6.642</v>
+        <v>6.64</v>
       </c>
     </row>
     <row r="38">
@@ -967,10 +967,10 @@
         <v>4.34</v>
       </c>
       <c r="C38" t="n">
-        <v>6.935</v>
+        <v>6.93</v>
       </c>
       <c r="D38" t="n">
-        <v>11.623</v>
+        <v>11.62</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>47</v>
       </c>
       <c r="B39" t="n">
-        <v>4.211</v>
+        <v>4.21</v>
       </c>
       <c r="C39" t="n">
-        <v>6.747</v>
+        <v>6.75</v>
       </c>
       <c r="D39" t="n">
-        <v>8.423</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>48</v>
       </c>
       <c r="B40" t="n">
-        <v>4.149</v>
+        <v>4.15</v>
       </c>
       <c r="C40" t="n">
-        <v>6.613</v>
+        <v>6.61</v>
       </c>
       <c r="D40" t="n">
-        <v>6.681</v>
+        <v>6.68</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>49</v>
       </c>
       <c r="B41" t="n">
-        <v>5.089</v>
+        <v>5.09</v>
       </c>
       <c r="C41" t="n">
-        <v>8.175000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="D41" t="n">
-        <v>8.686</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>4.253</v>
+        <v>4.25</v>
       </c>
       <c r="C42" t="n">
-        <v>6.761</v>
+        <v>6.76</v>
       </c>
       <c r="D42" t="n">
-        <v>8.506</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>3.649</v>
+        <v>3.65</v>
       </c>
       <c r="C43" t="n">
-        <v>5.757</v>
+        <v>5.76</v>
       </c>
       <c r="D43" t="n">
-        <v>2.854</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>52</v>
       </c>
       <c r="B44" t="n">
-        <v>4.258</v>
+        <v>4.26</v>
       </c>
       <c r="C44" t="n">
-        <v>6.762</v>
+        <v>6.76</v>
       </c>
       <c r="D44" t="n">
-        <v>8.516</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>53</v>
       </c>
       <c r="B45" t="n">
-        <v>4.258</v>
+        <v>4.26</v>
       </c>
       <c r="C45" t="n">
-        <v>6.757</v>
+        <v>6.76</v>
       </c>
       <c r="D45" t="n">
-        <v>8.516</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>54</v>
       </c>
       <c r="B46" t="n">
-        <v>4.258</v>
+        <v>4.26</v>
       </c>
       <c r="C46" t="n">
-        <v>6.762</v>
+        <v>6.76</v>
       </c>
       <c r="D46" t="n">
-        <v>8.516</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>55</v>
       </c>
       <c r="B47" t="n">
-        <v>3.649</v>
+        <v>3.65</v>
       </c>
       <c r="C47" t="n">
-        <v>5.757</v>
+        <v>5.76</v>
       </c>
       <c r="D47" t="n">
-        <v>2.854</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>56</v>
       </c>
       <c r="B48" t="n">
-        <v>4.253</v>
+        <v>4.25</v>
       </c>
       <c r="C48" t="n">
-        <v>6.761</v>
+        <v>6.76</v>
       </c>
       <c r="D48" t="n">
-        <v>8.506</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>57</v>
       </c>
       <c r="B49" t="n">
-        <v>5.089</v>
+        <v>5.09</v>
       </c>
       <c r="C49" t="n">
-        <v>8.175000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="D49" t="n">
-        <v>8.686</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>58</v>
       </c>
       <c r="B50" t="n">
-        <v>4.149</v>
+        <v>4.15</v>
       </c>
       <c r="C50" t="n">
-        <v>6.613</v>
+        <v>6.61</v>
       </c>
       <c r="D50" t="n">
-        <v>6.681</v>
+        <v>6.68</v>
       </c>
     </row>
     <row r="51">
@@ -1146,13 +1146,13 @@
         <v>59</v>
       </c>
       <c r="B51" t="n">
-        <v>4.211</v>
+        <v>4.21</v>
       </c>
       <c r="C51" t="n">
-        <v>6.747</v>
+        <v>6.75</v>
       </c>
       <c r="D51" t="n">
-        <v>8.423</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="52">
@@ -1163,10 +1163,10 @@
         <v>4.34</v>
       </c>
       <c r="C52" t="n">
-        <v>6.935</v>
+        <v>6.93</v>
       </c>
       <c r="D52" t="n">
-        <v>11.623</v>
+        <v>11.62</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>61</v>
       </c>
       <c r="B53" t="n">
-        <v>4.149</v>
+        <v>4.15</v>
       </c>
       <c r="C53" t="n">
-        <v>6.564</v>
+        <v>6.56</v>
       </c>
       <c r="D53" t="n">
-        <v>6.642</v>
+        <v>6.64</v>
       </c>
     </row>
     <row r="54">
@@ -1188,10 +1188,10 @@
         <v>62</v>
       </c>
       <c r="B54" t="n">
-        <v>4.145</v>
+        <v>4.15</v>
       </c>
       <c r="C54" t="n">
-        <v>6.548</v>
+        <v>6.55</v>
       </c>
       <c r="D54" t="n">
         <v>8.289999999999999</v>
@@ -1202,13 +1202,13 @@
         <v>63</v>
       </c>
       <c r="B55" t="n">
-        <v>4.346</v>
+        <v>4.35</v>
       </c>
       <c r="C55" t="n">
-        <v>6.892</v>
+        <v>6.89</v>
       </c>
       <c r="D55" t="n">
-        <v>11.766</v>
+        <v>11.77</v>
       </c>
     </row>
     <row r="56">
@@ -1216,13 +1216,13 @@
         <v>64</v>
       </c>
       <c r="B56" t="n">
-        <v>4.434</v>
+        <v>4.43</v>
       </c>
       <c r="C56" t="n">
         <v>6.14</v>
       </c>
       <c r="D56" t="n">
-        <v>7.788</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="57">
@@ -1230,13 +1230,13 @@
         <v>65</v>
       </c>
       <c r="B57" t="n">
-        <v>5.005</v>
+        <v>5</v>
       </c>
       <c r="C57" t="n">
-        <v>5.985</v>
+        <v>5.98</v>
       </c>
       <c r="D57" t="n">
-        <v>10.009</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="58">
@@ -1244,13 +1244,13 @@
         <v>66</v>
       </c>
       <c r="B58" t="n">
-        <v>4.549</v>
+        <v>4.55</v>
       </c>
       <c r="C58" t="n">
-        <v>6.285</v>
+        <v>6.28</v>
       </c>
       <c r="D58" t="n">
-        <v>10.607</v>
+        <v>10.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add final data for fabian
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_d.xlsx
+++ b/data/fabian/output/processed_d.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,60 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>sigmaYZ</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaXZ</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaZZ</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Load Case 1 RF</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaYZ</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaXZ</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaZZ</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Load Case 2 RF</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaYZ</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaXZ</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>sigmaZZ</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Load Case 3 RF</t>
         </is>
@@ -460,12 +505,39 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>4.07</v>
       </c>
-      <c r="C2" t="n">
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>6.91</v>
       </c>
-      <c r="D2" t="n">
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
         <v>1.09</v>
       </c>
     </row>
@@ -474,12 +546,39 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
         <v>3.33</v>
       </c>
-      <c r="C3" t="n">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>5.93</v>
       </c>
-      <c r="D3" t="n">
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
         <v>1.24</v>
       </c>
     </row>
@@ -488,12 +587,39 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>3.45</v>
       </c>
-      <c r="C4" t="n">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>6.02</v>
       </c>
-      <c r="D4" t="n">
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>1.04</v>
       </c>
     </row>
@@ -502,12 +628,39 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>3.06</v>
       </c>
-      <c r="C5" t="n">
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>5.17</v>
       </c>
-      <c r="D5" t="n">
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>1.05</v>
       </c>
     </row>
@@ -516,12 +669,39 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
         <v>3.09</v>
       </c>
-      <c r="C6" t="n">
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
         <v>5.6</v>
       </c>
-      <c r="D6" t="n">
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
         <v>1.24</v>
       </c>
     </row>
@@ -530,12 +710,39 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>2.89</v>
       </c>
-      <c r="C7" t="n">
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>5.08</v>
       </c>
-      <c r="D7" t="n">
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
         <v>1.03</v>
       </c>
     </row>
@@ -544,12 +751,39 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
         <v>3.23</v>
       </c>
-      <c r="C8" t="n">
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
         <v>5.3</v>
       </c>
-      <c r="D8" t="n">
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
         <v>1.03</v>
       </c>
     </row>
@@ -558,12 +792,39 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>3.02</v>
       </c>
-      <c r="C9" t="n">
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
         <v>5.3</v>
       </c>
-      <c r="D9" t="n">
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>1.25</v>
       </c>
     </row>
@@ -572,12 +833,39 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
         <v>2.77</v>
       </c>
-      <c r="C10" t="n">
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>4.93</v>
       </c>
-      <c r="D10" t="n">
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
         <v>0.97</v>
       </c>
     </row>
@@ -586,12 +874,39 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
         <v>3.44</v>
       </c>
-      <c r="C11" t="n">
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
         <v>5.44</v>
       </c>
-      <c r="D11" t="n">
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
         <v>0.89</v>
       </c>
     </row>
@@ -600,12 +915,39 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
         <v>3.18</v>
       </c>
-      <c r="C12" t="n">
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
         <v>5.59</v>
       </c>
-      <c r="D12" t="n">
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>1.53</v>
       </c>
     </row>
@@ -614,12 +956,39 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
         <v>2.47</v>
       </c>
-      <c r="C13" t="n">
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
         <v>4.36</v>
       </c>
-      <c r="D13" t="n">
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
         <v>0.82</v>
       </c>
     </row>
@@ -628,12 +997,39 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
         <v>2.67</v>
       </c>
-      <c r="C14" t="n">
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
         <v>4.28</v>
       </c>
-      <c r="D14" t="n">
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -642,12 +1038,39 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
         <v>2.69</v>
       </c>
-      <c r="C15" t="n">
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
         <v>4.51</v>
       </c>
-      <c r="D15" t="n">
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
         <v>0.73</v>
       </c>
     </row>
@@ -656,12 +1079,39 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
         <v>2.28</v>
       </c>
-      <c r="C16" t="n">
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>3.82</v>
       </c>
-      <c r="D16" t="n">
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>0.58</v>
       </c>
     </row>
@@ -670,12 +1120,39 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
         <v>2.28</v>
       </c>
-      <c r="C17" t="n">
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
         <v>3.82</v>
       </c>
-      <c r="D17" t="n">
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
         <v>0.58</v>
       </c>
     </row>
@@ -684,12 +1161,39 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
         <v>2.69</v>
       </c>
-      <c r="C18" t="n">
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
         <v>4.51</v>
       </c>
-      <c r="D18" t="n">
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
         <v>0.73</v>
       </c>
     </row>
@@ -698,12 +1202,39 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
         <v>2.67</v>
       </c>
-      <c r="C19" t="n">
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
         <v>4.28</v>
       </c>
-      <c r="D19" t="n">
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -712,12 +1243,39 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
         <v>2.47</v>
       </c>
-      <c r="C20" t="n">
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
         <v>4.36</v>
       </c>
-      <c r="D20" t="n">
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
         <v>0.82</v>
       </c>
     </row>
@@ -726,12 +1284,39 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
         <v>3.18</v>
       </c>
-      <c r="C21" t="n">
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
         <v>5.59</v>
       </c>
-      <c r="D21" t="n">
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
         <v>1.53</v>
       </c>
     </row>
@@ -740,12 +1325,39 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
         <v>3.44</v>
       </c>
-      <c r="C22" t="n">
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
         <v>5.44</v>
       </c>
-      <c r="D22" t="n">
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
         <v>0.89</v>
       </c>
     </row>
@@ -754,12 +1366,39 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
         <v>2.77</v>
       </c>
-      <c r="C23" t="n">
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
         <v>4.93</v>
       </c>
-      <c r="D23" t="n">
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
         <v>0.97</v>
       </c>
     </row>
@@ -768,12 +1407,39 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
         <v>3.02</v>
       </c>
-      <c r="C24" t="n">
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
         <v>5.3</v>
       </c>
-      <c r="D24" t="n">
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
         <v>1.25</v>
       </c>
     </row>
@@ -782,12 +1448,39 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
         <v>3.23</v>
       </c>
-      <c r="C25" t="n">
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
         <v>5.3</v>
       </c>
-      <c r="D25" t="n">
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
         <v>1.03</v>
       </c>
     </row>
@@ -796,12 +1489,39 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
         <v>2.89</v>
       </c>
-      <c r="C26" t="n">
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
         <v>5.08</v>
       </c>
-      <c r="D26" t="n">
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
         <v>1.03</v>
       </c>
     </row>
@@ -810,12 +1530,39 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
         <v>3.09</v>
       </c>
-      <c r="C27" t="n">
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
         <v>5.6</v>
       </c>
-      <c r="D27" t="n">
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
         <v>1.24</v>
       </c>
     </row>
@@ -824,12 +1571,39 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
         <v>3.06</v>
       </c>
-      <c r="C28" t="n">
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
         <v>5.17</v>
       </c>
-      <c r="D28" t="n">
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
         <v>1.05</v>
       </c>
     </row>
@@ -838,12 +1612,39 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
         <v>3.45</v>
       </c>
-      <c r="C29" t="n">
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
         <v>6.02</v>
       </c>
-      <c r="D29" t="n">
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
         <v>1.04</v>
       </c>
     </row>
@@ -852,12 +1653,39 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
         <v>3.33</v>
       </c>
-      <c r="C30" t="n">
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
         <v>5.93</v>
       </c>
-      <c r="D30" t="n">
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
         <v>1.24</v>
       </c>
     </row>
@@ -866,12 +1694,39 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
         <v>4.07</v>
       </c>
-      <c r="C31" t="n">
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
         <v>6.91</v>
       </c>
-      <c r="D31" t="n">
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
         <v>1.09</v>
       </c>
     </row>
@@ -879,13 +1734,22 @@
       <c r="A32" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="n">
         <v>4.55</v>
       </c>
-      <c r="C32" t="n">
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="n">
         <v>6.28</v>
       </c>
-      <c r="D32" t="n">
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="n">
         <v>10.61</v>
       </c>
     </row>
@@ -893,13 +1757,22 @@
       <c r="A33" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
         <v>5</v>
       </c>
-      <c r="C33" t="n">
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="n">
         <v>5.98</v>
       </c>
-      <c r="D33" t="n">
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="n">
         <v>10.01</v>
       </c>
     </row>
@@ -907,13 +1780,22 @@
       <c r="A34" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="n">
         <v>4.43</v>
       </c>
-      <c r="C34" t="n">
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="n">
         <v>6.14</v>
       </c>
-      <c r="D34" t="n">
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="n">
         <v>7.79</v>
       </c>
     </row>
@@ -921,13 +1803,22 @@
       <c r="A35" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="n">
         <v>4.35</v>
       </c>
-      <c r="C35" t="n">
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="n">
         <v>6.89</v>
       </c>
-      <c r="D35" t="n">
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="n">
         <v>11.77</v>
       </c>
     </row>
@@ -935,13 +1826,22 @@
       <c r="A36" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
         <v>4.15</v>
       </c>
-      <c r="C36" t="n">
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="n">
         <v>6.55</v>
       </c>
-      <c r="D36" t="n">
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="n">
         <v>8.289999999999999</v>
       </c>
     </row>
@@ -949,13 +1849,22 @@
       <c r="A37" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
         <v>4.15</v>
       </c>
-      <c r="C37" t="n">
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
         <v>6.56</v>
       </c>
-      <c r="D37" t="n">
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="n">
         <v>6.64</v>
       </c>
     </row>
@@ -963,13 +1872,22 @@
       <c r="A38" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="n">
         <v>4.34</v>
       </c>
-      <c r="C38" t="n">
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
         <v>6.93</v>
       </c>
-      <c r="D38" t="n">
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="n">
         <v>11.62</v>
       </c>
     </row>
@@ -977,13 +1895,22 @@
       <c r="A39" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="n">
         <v>4.21</v>
       </c>
-      <c r="C39" t="n">
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
         <v>6.75</v>
       </c>
-      <c r="D39" t="n">
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="n">
         <v>8.42</v>
       </c>
     </row>
@@ -991,13 +1918,22 @@
       <c r="A40" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="n">
         <v>4.15</v>
       </c>
-      <c r="C40" t="n">
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
         <v>6.61</v>
       </c>
-      <c r="D40" t="n">
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="n">
         <v>6.68</v>
       </c>
     </row>
@@ -1005,13 +1941,22 @@
       <c r="A41" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="n">
         <v>5.09</v>
       </c>
-      <c r="C41" t="n">
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
         <v>8.18</v>
       </c>
-      <c r="D41" t="n">
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="n">
         <v>8.69</v>
       </c>
     </row>
@@ -1019,13 +1964,22 @@
       <c r="A42" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
         <v>4.25</v>
       </c>
-      <c r="C42" t="n">
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="n">
         <v>6.76</v>
       </c>
-      <c r="D42" t="n">
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="n">
         <v>8.51</v>
       </c>
     </row>
@@ -1033,13 +1987,22 @@
       <c r="A43" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="n">
         <v>3.65</v>
       </c>
-      <c r="C43" t="n">
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="n">
         <v>5.76</v>
       </c>
-      <c r="D43" t="n">
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="n">
         <v>2.85</v>
       </c>
     </row>
@@ -1047,13 +2010,22 @@
       <c r="A44" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="n">
         <v>4.26</v>
       </c>
-      <c r="C44" t="n">
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="n">
         <v>6.76</v>
       </c>
-      <c r="D44" t="n">
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="n">
         <v>8.52</v>
       </c>
     </row>
@@ -1061,13 +2033,22 @@
       <c r="A45" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="n">
         <v>4.26</v>
       </c>
-      <c r="C45" t="n">
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="n">
         <v>6.76</v>
       </c>
-      <c r="D45" t="n">
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="n">
         <v>8.52</v>
       </c>
     </row>
@@ -1075,13 +2056,22 @@
       <c r="A46" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="n">
         <v>4.26</v>
       </c>
-      <c r="C46" t="n">
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="n">
         <v>6.76</v>
       </c>
-      <c r="D46" t="n">
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="n">
         <v>8.52</v>
       </c>
     </row>
@@ -1089,13 +2079,22 @@
       <c r="A47" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="n">
         <v>3.65</v>
       </c>
-      <c r="C47" t="n">
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="n">
         <v>5.76</v>
       </c>
-      <c r="D47" t="n">
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="n">
         <v>2.85</v>
       </c>
     </row>
@@ -1103,13 +2102,22 @@
       <c r="A48" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="n">
         <v>4.25</v>
       </c>
-      <c r="C48" t="n">
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="n">
         <v>6.76</v>
       </c>
-      <c r="D48" t="n">
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="n">
         <v>8.51</v>
       </c>
     </row>
@@ -1117,13 +2125,22 @@
       <c r="A49" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="n">
         <v>5.09</v>
       </c>
-      <c r="C49" t="n">
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="n">
         <v>8.18</v>
       </c>
-      <c r="D49" t="n">
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="n">
         <v>8.69</v>
       </c>
     </row>
@@ -1131,13 +2148,22 @@
       <c r="A50" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="n">
         <v>4.15</v>
       </c>
-      <c r="C50" t="n">
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="n">
         <v>6.61</v>
       </c>
-      <c r="D50" t="n">
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="n">
         <v>6.68</v>
       </c>
     </row>
@@ -1145,13 +2171,22 @@
       <c r="A51" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
         <v>4.21</v>
       </c>
-      <c r="C51" t="n">
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="n">
         <v>6.75</v>
       </c>
-      <c r="D51" t="n">
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="n">
         <v>8.42</v>
       </c>
     </row>
@@ -1159,13 +2194,22 @@
       <c r="A52" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
         <v>4.34</v>
       </c>
-      <c r="C52" t="n">
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="n">
         <v>6.93</v>
       </c>
-      <c r="D52" t="n">
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="n">
         <v>11.62</v>
       </c>
     </row>
@@ -1173,13 +2217,22 @@
       <c r="A53" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="n">
         <v>4.15</v>
       </c>
-      <c r="C53" t="n">
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="n">
         <v>6.56</v>
       </c>
-      <c r="D53" t="n">
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="n">
         <v>6.64</v>
       </c>
     </row>
@@ -1187,13 +2240,22 @@
       <c r="A54" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="n">
         <v>4.15</v>
       </c>
-      <c r="C54" t="n">
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="n">
         <v>6.55</v>
       </c>
-      <c r="D54" t="n">
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="n">
         <v>8.289999999999999</v>
       </c>
     </row>
@@ -1201,13 +2263,22 @@
       <c r="A55" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
         <v>4.35</v>
       </c>
-      <c r="C55" t="n">
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="n">
         <v>6.89</v>
       </c>
-      <c r="D55" t="n">
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="n">
         <v>11.77</v>
       </c>
     </row>
@@ -1215,13 +2286,22 @@
       <c r="A56" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="n">
         <v>4.43</v>
       </c>
-      <c r="C56" t="n">
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="n">
         <v>6.14</v>
       </c>
-      <c r="D56" t="n">
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="n">
         <v>7.79</v>
       </c>
     </row>
@@ -1229,13 +2309,22 @@
       <c r="A57" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
         <v>5</v>
       </c>
-      <c r="C57" t="n">
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="n">
         <v>5.98</v>
       </c>
-      <c r="D57" t="n">
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="n">
         <v>10.01</v>
       </c>
     </row>
@@ -1243,13 +2332,22 @@
       <c r="A58" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
         <v>4.55</v>
       </c>
-      <c r="C58" t="n">
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="n">
         <v>6.28</v>
       </c>
-      <c r="D58" t="n">
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="n">
         <v>10.61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
increased rounding to 3 digits
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_d.xlsx
+++ b/data/fabian/output/processed_d.xlsx
@@ -460,13 +460,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4.07</v>
+        <v>4.074</v>
       </c>
       <c r="C2" t="n">
-        <v>6.91</v>
+        <v>4.575</v>
       </c>
       <c r="D2" t="n">
-        <v>1.09</v>
+        <v>1.642</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.33</v>
+        <v>3.331</v>
       </c>
       <c r="C3" t="n">
-        <v>5.93</v>
+        <v>3.927</v>
       </c>
       <c r="D3" t="n">
-        <v>1.24</v>
+        <v>1.868</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.45</v>
+        <v>3.447</v>
       </c>
       <c r="C4" t="n">
-        <v>6.02</v>
+        <v>3.986</v>
       </c>
       <c r="D4" t="n">
-        <v>1.04</v>
+        <v>1.577</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.06</v>
+        <v>3.057</v>
       </c>
       <c r="C5" t="n">
-        <v>5.17</v>
+        <v>3.427</v>
       </c>
       <c r="D5" t="n">
-        <v>1.05</v>
+        <v>1.591</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.09</v>
+        <v>3.085</v>
       </c>
       <c r="C6" t="n">
-        <v>5.6</v>
+        <v>3.709</v>
       </c>
       <c r="D6" t="n">
-        <v>1.24</v>
+        <v>1.866</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.89</v>
+        <v>2.888</v>
       </c>
       <c r="C7" t="n">
-        <v>5.08</v>
+        <v>3.363</v>
       </c>
       <c r="D7" t="n">
-        <v>1.03</v>
+        <v>1.558</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.23</v>
+        <v>3.232</v>
       </c>
       <c r="C8" t="n">
-        <v>5.3</v>
+        <v>3.513</v>
       </c>
       <c r="D8" t="n">
-        <v>1.03</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.02</v>
+        <v>3.016</v>
       </c>
       <c r="C9" t="n">
-        <v>5.3</v>
+        <v>3.509</v>
       </c>
       <c r="D9" t="n">
-        <v>1.25</v>
+        <v>1.881</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2.77</v>
+        <v>2.768</v>
       </c>
       <c r="C10" t="n">
-        <v>4.93</v>
+        <v>3.267</v>
       </c>
       <c r="D10" t="n">
-        <v>0.97</v>
+        <v>1.471</v>
       </c>
     </row>
     <row r="11">
@@ -589,10 +589,10 @@
         <v>3.44</v>
       </c>
       <c r="C11" t="n">
-        <v>5.44</v>
+        <v>3.602</v>
       </c>
       <c r="D11" t="n">
-        <v>0.89</v>
+        <v>1.345</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3.18</v>
+        <v>3.178</v>
       </c>
       <c r="C12" t="n">
-        <v>5.59</v>
+        <v>3.702</v>
       </c>
       <c r="D12" t="n">
-        <v>1.53</v>
+        <v>2.314</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2.47</v>
+        <v>2.469</v>
       </c>
       <c r="C13" t="n">
-        <v>4.36</v>
+        <v>2.888</v>
       </c>
       <c r="D13" t="n">
-        <v>0.82</v>
+        <v>1.234</v>
       </c>
     </row>
     <row r="14">
@@ -631,10 +631,10 @@
         <v>2.67</v>
       </c>
       <c r="C14" t="n">
-        <v>4.28</v>
+        <v>2.837</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6</v>
+        <v>0.899</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.69</v>
+        <v>2.694</v>
       </c>
       <c r="C15" t="n">
-        <v>4.51</v>
+        <v>2.985</v>
       </c>
       <c r="D15" t="n">
-        <v>0.73</v>
+        <v>1.101</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.28</v>
+        <v>2.283</v>
       </c>
       <c r="C16" t="n">
-        <v>3.82</v>
+        <v>2.529</v>
       </c>
       <c r="D16" t="n">
-        <v>0.58</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.28</v>
+        <v>2.283</v>
       </c>
       <c r="C17" t="n">
-        <v>3.82</v>
+        <v>2.529</v>
       </c>
       <c r="D17" t="n">
-        <v>0.58</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.69</v>
+        <v>2.694</v>
       </c>
       <c r="C18" t="n">
-        <v>4.51</v>
+        <v>2.985</v>
       </c>
       <c r="D18" t="n">
-        <v>0.73</v>
+        <v>1.101</v>
       </c>
     </row>
     <row r="19">
@@ -701,10 +701,10 @@
         <v>2.67</v>
       </c>
       <c r="C19" t="n">
-        <v>4.28</v>
+        <v>2.837</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6</v>
+        <v>0.899</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.47</v>
+        <v>2.469</v>
       </c>
       <c r="C20" t="n">
-        <v>4.36</v>
+        <v>2.888</v>
       </c>
       <c r="D20" t="n">
-        <v>0.82</v>
+        <v>1.234</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>3.18</v>
+        <v>3.178</v>
       </c>
       <c r="C21" t="n">
-        <v>5.59</v>
+        <v>3.702</v>
       </c>
       <c r="D21" t="n">
-        <v>1.53</v>
+        <v>2.314</v>
       </c>
     </row>
     <row r="22">
@@ -743,10 +743,10 @@
         <v>3.44</v>
       </c>
       <c r="C22" t="n">
-        <v>5.44</v>
+        <v>3.602</v>
       </c>
       <c r="D22" t="n">
-        <v>0.89</v>
+        <v>1.345</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2.77</v>
+        <v>2.768</v>
       </c>
       <c r="C23" t="n">
-        <v>4.93</v>
+        <v>3.267</v>
       </c>
       <c r="D23" t="n">
-        <v>0.97</v>
+        <v>1.471</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>3.02</v>
+        <v>3.016</v>
       </c>
       <c r="C24" t="n">
-        <v>5.3</v>
+        <v>3.509</v>
       </c>
       <c r="D24" t="n">
-        <v>1.25</v>
+        <v>1.881</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.23</v>
+        <v>3.232</v>
       </c>
       <c r="C25" t="n">
-        <v>5.3</v>
+        <v>3.513</v>
       </c>
       <c r="D25" t="n">
-        <v>1.03</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2.89</v>
+        <v>2.888</v>
       </c>
       <c r="C26" t="n">
-        <v>5.08</v>
+        <v>3.363</v>
       </c>
       <c r="D26" t="n">
-        <v>1.03</v>
+        <v>1.558</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.09</v>
+        <v>3.085</v>
       </c>
       <c r="C27" t="n">
-        <v>5.6</v>
+        <v>3.709</v>
       </c>
       <c r="D27" t="n">
-        <v>1.24</v>
+        <v>1.866</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3.06</v>
+        <v>3.057</v>
       </c>
       <c r="C28" t="n">
-        <v>5.17</v>
+        <v>3.427</v>
       </c>
       <c r="D28" t="n">
-        <v>1.05</v>
+        <v>1.591</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>3.45</v>
+        <v>3.447</v>
       </c>
       <c r="C29" t="n">
-        <v>6.02</v>
+        <v>3.986</v>
       </c>
       <c r="D29" t="n">
-        <v>1.04</v>
+        <v>1.577</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>3.33</v>
+        <v>3.331</v>
       </c>
       <c r="C30" t="n">
-        <v>5.93</v>
+        <v>3.927</v>
       </c>
       <c r="D30" t="n">
-        <v>1.24</v>
+        <v>1.868</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>4.07</v>
+        <v>4.074</v>
       </c>
       <c r="C31" t="n">
-        <v>6.91</v>
+        <v>4.575</v>
       </c>
       <c r="D31" t="n">
-        <v>1.09</v>
+        <v>1.642</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>4.55</v>
+        <v>4.549</v>
       </c>
       <c r="C32" t="n">
-        <v>6.28</v>
+        <v>4.162</v>
       </c>
       <c r="D32" t="n">
-        <v>10.61</v>
+        <v>16.018</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>5.004</v>
       </c>
       <c r="C33" t="n">
-        <v>5.98</v>
+        <v>3.963</v>
       </c>
       <c r="D33" t="n">
-        <v>10.01</v>
+        <v>15.113</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>42</v>
       </c>
       <c r="B34" t="n">
-        <v>4.43</v>
+        <v>4.434</v>
       </c>
       <c r="C34" t="n">
-        <v>6.14</v>
+        <v>4.066</v>
       </c>
       <c r="D34" t="n">
-        <v>7.79</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>4.35</v>
+        <v>4.346</v>
       </c>
       <c r="C35" t="n">
-        <v>6.89</v>
+        <v>4.564</v>
       </c>
       <c r="D35" t="n">
-        <v>11.77</v>
+        <v>17.766</v>
       </c>
     </row>
     <row r="36">
@@ -936,13 +936,13 @@
         <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>4.15</v>
+        <v>4.145</v>
       </c>
       <c r="C36" t="n">
-        <v>6.55</v>
+        <v>4.336</v>
       </c>
       <c r="D36" t="n">
-        <v>8.289999999999999</v>
+        <v>12.518</v>
       </c>
     </row>
     <row r="37">
@@ -950,13 +950,13 @@
         <v>45</v>
       </c>
       <c r="B37" t="n">
-        <v>4.15</v>
+        <v>4.149</v>
       </c>
       <c r="C37" t="n">
-        <v>6.56</v>
+        <v>4.347</v>
       </c>
       <c r="D37" t="n">
-        <v>6.64</v>
+        <v>10.029</v>
       </c>
     </row>
     <row r="38">
@@ -964,13 +964,13 @@
         <v>46</v>
       </c>
       <c r="B38" t="n">
-        <v>4.34</v>
+        <v>4.339</v>
       </c>
       <c r="C38" t="n">
-        <v>6.93</v>
+        <v>4.593</v>
       </c>
       <c r="D38" t="n">
-        <v>11.62</v>
+        <v>17.548</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>47</v>
       </c>
       <c r="B39" t="n">
-        <v>4.21</v>
+        <v>4.211</v>
       </c>
       <c r="C39" t="n">
-        <v>6.75</v>
+        <v>4.468</v>
       </c>
       <c r="D39" t="n">
-        <v>8.42</v>
+        <v>12.717</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>48</v>
       </c>
       <c r="B40" t="n">
-        <v>4.15</v>
+        <v>4.149</v>
       </c>
       <c r="C40" t="n">
-        <v>6.61</v>
+        <v>4.379</v>
       </c>
       <c r="D40" t="n">
-        <v>6.68</v>
+        <v>10.087</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>49</v>
       </c>
       <c r="B41" t="n">
-        <v>5.09</v>
+        <v>5.089</v>
       </c>
       <c r="C41" t="n">
-        <v>8.18</v>
+        <v>5.414</v>
       </c>
       <c r="D41" t="n">
-        <v>8.69</v>
+        <v>13.116</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>4.25</v>
+        <v>4.253</v>
       </c>
       <c r="C42" t="n">
-        <v>6.76</v>
+        <v>4.478</v>
       </c>
       <c r="D42" t="n">
-        <v>8.51</v>
+        <v>12.843</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>3.65</v>
+        <v>3.649</v>
       </c>
       <c r="C43" t="n">
-        <v>5.76</v>
+        <v>3.813</v>
       </c>
       <c r="D43" t="n">
-        <v>2.85</v>
+        <v>4.309</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>52</v>
       </c>
       <c r="B44" t="n">
-        <v>4.26</v>
+        <v>4.258</v>
       </c>
       <c r="C44" t="n">
-        <v>6.76</v>
+        <v>4.478</v>
       </c>
       <c r="D44" t="n">
-        <v>8.52</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>53</v>
       </c>
       <c r="B45" t="n">
-        <v>4.26</v>
+        <v>4.258</v>
       </c>
       <c r="C45" t="n">
-        <v>6.76</v>
+        <v>4.475</v>
       </c>
       <c r="D45" t="n">
-        <v>8.52</v>
+        <v>12.858</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>54</v>
       </c>
       <c r="B46" t="n">
-        <v>4.26</v>
+        <v>4.258</v>
       </c>
       <c r="C46" t="n">
-        <v>6.76</v>
+        <v>4.478</v>
       </c>
       <c r="D46" t="n">
-        <v>8.52</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>55</v>
       </c>
       <c r="B47" t="n">
-        <v>3.65</v>
+        <v>3.649</v>
       </c>
       <c r="C47" t="n">
-        <v>5.76</v>
+        <v>3.813</v>
       </c>
       <c r="D47" t="n">
-        <v>2.85</v>
+        <v>4.309</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>56</v>
       </c>
       <c r="B48" t="n">
-        <v>4.25</v>
+        <v>4.253</v>
       </c>
       <c r="C48" t="n">
-        <v>6.76</v>
+        <v>4.478</v>
       </c>
       <c r="D48" t="n">
-        <v>8.51</v>
+        <v>12.843</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>57</v>
       </c>
       <c r="B49" t="n">
-        <v>5.09</v>
+        <v>5.089</v>
       </c>
       <c r="C49" t="n">
-        <v>8.18</v>
+        <v>5.414</v>
       </c>
       <c r="D49" t="n">
-        <v>8.69</v>
+        <v>13.116</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>58</v>
       </c>
       <c r="B50" t="n">
-        <v>4.15</v>
+        <v>4.149</v>
       </c>
       <c r="C50" t="n">
-        <v>6.61</v>
+        <v>4.379</v>
       </c>
       <c r="D50" t="n">
-        <v>6.68</v>
+        <v>10.087</v>
       </c>
     </row>
     <row r="51">
@@ -1146,13 +1146,13 @@
         <v>59</v>
       </c>
       <c r="B51" t="n">
-        <v>4.21</v>
+        <v>4.211</v>
       </c>
       <c r="C51" t="n">
-        <v>6.75</v>
+        <v>4.468</v>
       </c>
       <c r="D51" t="n">
-        <v>8.42</v>
+        <v>12.717</v>
       </c>
     </row>
     <row r="52">
@@ -1160,13 +1160,13 @@
         <v>60</v>
       </c>
       <c r="B52" t="n">
-        <v>4.34</v>
+        <v>4.339</v>
       </c>
       <c r="C52" t="n">
-        <v>6.93</v>
+        <v>4.593</v>
       </c>
       <c r="D52" t="n">
-        <v>11.62</v>
+        <v>17.548</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>61</v>
       </c>
       <c r="B53" t="n">
-        <v>4.15</v>
+        <v>4.149</v>
       </c>
       <c r="C53" t="n">
-        <v>6.56</v>
+        <v>4.347</v>
       </c>
       <c r="D53" t="n">
-        <v>6.64</v>
+        <v>10.029</v>
       </c>
     </row>
     <row r="54">
@@ -1188,13 +1188,13 @@
         <v>62</v>
       </c>
       <c r="B54" t="n">
-        <v>4.15</v>
+        <v>4.145</v>
       </c>
       <c r="C54" t="n">
-        <v>6.55</v>
+        <v>4.336</v>
       </c>
       <c r="D54" t="n">
-        <v>8.289999999999999</v>
+        <v>12.518</v>
       </c>
     </row>
     <row r="55">
@@ -1202,13 +1202,13 @@
         <v>63</v>
       </c>
       <c r="B55" t="n">
-        <v>4.35</v>
+        <v>4.346</v>
       </c>
       <c r="C55" t="n">
-        <v>6.89</v>
+        <v>4.564</v>
       </c>
       <c r="D55" t="n">
-        <v>11.77</v>
+        <v>17.766</v>
       </c>
     </row>
     <row r="56">
@@ -1216,13 +1216,13 @@
         <v>64</v>
       </c>
       <c r="B56" t="n">
-        <v>4.43</v>
+        <v>4.434</v>
       </c>
       <c r="C56" t="n">
-        <v>6.14</v>
+        <v>4.066</v>
       </c>
       <c r="D56" t="n">
-        <v>7.79</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="57">
@@ -1230,13 +1230,13 @@
         <v>65</v>
       </c>
       <c r="B57" t="n">
-        <v>5</v>
+        <v>5.004</v>
       </c>
       <c r="C57" t="n">
-        <v>5.98</v>
+        <v>3.963</v>
       </c>
       <c r="D57" t="n">
-        <v>10.01</v>
+        <v>15.113</v>
       </c>
     </row>
     <row r="58">
@@ -1244,13 +1244,13 @@
         <v>66</v>
       </c>
       <c r="B58" t="n">
-        <v>4.55</v>
+        <v>4.549</v>
       </c>
       <c r="C58" t="n">
-        <v>6.28</v>
+        <v>4.162</v>
       </c>
       <c r="D58" t="n">
-        <v>10.61</v>
+        <v>16.018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>